<commit_message>
nb: merging dataframe of start and stop frame
</commit_message>
<xml_diff>
--- a/notebooks/export/rce_per_subject_start_stop_video_frame.xlsx
+++ b/notebooks/export/rce_per_subject_start_stop_video_frame.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27321"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="233" documentId="11_62D7479E5772F09A29C9EFE5FCBFF434EA66B218" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{676375D5-7C1E-475F-8125-436A97B16680}"/>
+  <xr:revisionPtr revIDLastSave="236" documentId="11_62D7479E5772F09A29C9EFE5FCBFF434EA66B218" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C312C965-E30C-47AF-A7A0-FDD1570B5576}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,10 +42,10 @@
     <t>stop_frame</t>
   </si>
   <si>
-    <t>individual_subj</t>
-  </si>
-  <si>
-    <t>all_subj</t>
+    <t>tracked_subject</t>
+  </si>
+  <si>
+    <t>in_video_subjects</t>
   </si>
   <si>
     <t>notes</t>
@@ -536,8 +536,8 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D39" sqref="D39"/>
+      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1150,15 +1150,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101002C00C86E44419345A6E3C05C9040286D" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="18d96e1ddddca0bcf95d5c548c97f8cd">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="05f64c5e-7ec2-4cf0-a148-a77e53878df3" xmlns:ns3="66c7fa70-bb82-47de-8c9f-8b3ecea6303f" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="55a175e9096d6108dc88a010d5822697" ns2:_="" ns3:_="">
     <xsd:import namespace="05f64c5e-7ec2-4cf0-a148-a77e53878df3"/>
@@ -1413,7 +1404,7 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="66c7fa70-bb82-47de-8c9f-8b3ecea6303f" xsi:nil="true"/>
@@ -1424,14 +1415,23 @@
 </p:properties>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D770834-2B26-4F25-8CBB-FA13B41D6738}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A2E4F11-7516-4015-A04F-C6297B95747E}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A2E4F11-7516-4015-A04F-C6297B95747E}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AE888698-F550-4D99-B643-806A083D1CEB}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AE888698-F550-4D99-B643-806A083D1CEB}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D770834-2B26-4F25-8CBB-FA13B41D6738}"/>
 </file>
</xml_diff>

<commit_message>
nb: change to omission files
</commit_message>
<xml_diff>
--- a/notebooks/export/rce_per_subject_start_stop_video_frame.xlsx
+++ b/notebooks/export/rce_per_subject_start_stop_video_frame.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27321"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="236" documentId="11_62D7479E5772F09A29C9EFE5FCBFF434EA66B218" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C312C965-E30C-47AF-A7A0-FDD1570B5576}"/>
+  <xr:revisionPtr revIDLastSave="255" documentId="11_62D7479E5772F09A29C9EFE5FCBFF434EA66B218" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{86596137-42D4-46EE-B069-327B7C71BFAA}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -51,73 +51,73 @@
     <t>notes</t>
   </si>
   <si>
-    <t>/scratch/back_up/reward_competition_extention/proc/id_corrected/20221214_125409_om_and_comp_6_1_and_6_3/20221214_125409_om_and_comp_6_1_and_6_3.1.fixed.1_subj.round_1.id_corrected.h5</t>
+    <t>/scratch/back_up/reward_competition_extention/final_proc/id_corrected/20221214_125409_om_and_comp_6_1_and_6_3/20221214_125409_om_and_comp_6_1_and_6_3.1.fixed.1_subj.round_1.id_corrected.h5</t>
   </si>
   <si>
     <t>6.1_6.3</t>
   </si>
   <si>
-    <t>/scratch/back_up/reward_competition_extention/proc/id_corrected/20221214_125409_om_and_comp_6_1_and_6_3/20221214_125409_om_and_comp_6_1_and_6_3.1.fixed.2_subj.round_1.id_corrected.h5</t>
-  </si>
-  <si>
-    <t>/scratch/back_up/reward_competition_extention/proc/id_corrected/20221215_145401_comp_amd_om_6_1_and_6_3/20221215_145401_comp_amd_om_6_1_and_6_3.1.fixed.1_subj.round_1.id_corrected.h5</t>
-  </si>
-  <si>
-    <t>/scratch/back_up/reward_competition_extention/proc/id_corrected/20221215_145401_comp_amd_om_6_1_and_6_3/20221215_145401_comp_amd_om_6_1_and_6_3.1.fixed.2_subj.round_1.id_corrected.h5</t>
-  </si>
-  <si>
-    <t>/scratch/back_up/reward_competition_extention/proc/id_corrected/20230617_115521_standard_comp_to_omission_D1_subj_1-1_and_1-2/20230617_115521_standard_comp_to_omission_D1_subj_1-1_and_1-2.1.fixed.1_subj.round_1.id_corrected.h5</t>
+    <t>/scratch/back_up/reward_competition_extention/final_proc/id_corrected/20221214_125409_om_and_comp_6_1_and_6_3/20221214_125409_om_and_comp_6_1_and_6_3.1.fixed.2_subj.round_1.id_corrected.h5</t>
+  </si>
+  <si>
+    <t>/scratch/back_up/reward_competition_extention/final_proc/id_corrected/20221215_145401_comp_amd_om_6_1_and_6_3/20221215_145401_comp_amd_om_6_1_and_6_3.1.fixed.1_subj.round_1.id_corrected.h5</t>
+  </si>
+  <si>
+    <t>/scratch/back_up/reward_competition_extention/final_proc/id_corrected/20221215_145401_comp_amd_om_6_1_and_6_3/20221215_145401_comp_amd_om_6_1_and_6_3.1.fixed.2_subj.round_1.id_corrected.h5</t>
+  </si>
+  <si>
+    <t>/scratch/back_up/reward_competition_extention/final_proc/id_corrected/20230617_115521_standard_comp_to_omission_D1_subj_1-1_and_1-2/20230617_115521_standard_comp_to_omission_D1_subj_1-1_and_1-2.1.fixed.1_subj.round_1.id_corrected.h5</t>
   </si>
   <si>
     <t>1.1_1.2</t>
   </si>
   <si>
-    <t>/scratch/back_up/reward_competition_extention/proc/id_corrected/20230617_115521_standard_comp_to_omission_D1_subj_1-1_and_1-2/20230617_115521_standard_comp_to_omission_D1_subj_1-1_and_1-2.1.fixed.2_subj.round_1.id_corrected.h5</t>
-  </si>
-  <si>
-    <t>/scratch/back_up/reward_competition_extention/proc/id_corrected/20230617_115521_standard_comp_to_omission_D1_subj_1-1_and_1-2/20230617_115521_standard_comp_to_omission_D1_subj_1-1_and_1-2.3.fixed.1_subj.round_1.id_corrected.h5</t>
-  </si>
-  <si>
-    <t>/scratch/back_up/reward_competition_extention/proc/id_corrected/20230618_100636_standard_comp_to_omission_D2_subj_1-4_and_1-1/20230618_100636_standard_comp_to_omission_D2_subj_1-4_and_1-1.1.fixed.1_subj.round_1.id_corrected.h5</t>
+    <t>/scratch/back_up/reward_competition_extention/final_proc/id_corrected/20230617_115521_standard_comp_to_omission_D1_subj_1-1_and_1-2/20230617_115521_standard_comp_to_omission_D1_subj_1-1_and_1-2.1.fixed.2_subj.round_1.id_corrected.h5</t>
+  </si>
+  <si>
+    <t>/scratch/back_up/reward_competition_extention/final_proc/id_corrected/20230617_115521_standard_comp_to_omission_D1_subj_1-1_and_1-2/20230617_115521_standard_comp_to_omission_D1_subj_1-1_and_1-2.3.fixed.1_subj.round_1.id_corrected.h5</t>
+  </si>
+  <si>
+    <t>/scratch/back_up/reward_competition_extention/final_proc/id_corrected/20230618_100636_standard_comp_to_omission_D2_subj_1-4_and_1-1/20230618_100636_standard_comp_to_omission_D2_subj_1-4_and_1-1.1.fixed.1_subj.round_1.id_corrected.h5</t>
   </si>
   <si>
     <t>1.1_1.4</t>
   </si>
   <si>
-    <t>/scratch/back_up/reward_competition_extention/proc/id_corrected/20230618_100636_standard_comp_to_omission_D2_subj_1-4_and_1-1/20230618_100636_standard_comp_to_omission_D2_subj_1-4_and_1-1.1.fixed.2_subj.round_1.id_corrected.h5</t>
-  </si>
-  <si>
-    <t>/scratch/back_up/reward_competition_extention/proc/id_corrected/20230618_100636_standard_comp_to_omission_D2_subj_1-4_and_1-1/20230618_100636_standard_comp_to_omission_D2_subj_1-4_and_1-1.2.fixed.1_subj.round_1.id_corrected.h5</t>
-  </si>
-  <si>
-    <t>/scratch/back_up/reward_competition_extention/proc/id_corrected/20230619_115321_standard_comp_to_omission_D3_subj_1-2_and_1-4/20230619_115321_standard_comp_to_omission_D3_subj_1-2_and_1-4.3.fixed.1_subj.round_1.id_corrected.h5</t>
+    <t>/scratch/back_up/reward_competition_extention/final_proc/id_corrected/20230618_100636_standard_comp_to_omission_D2_subj_1-4_and_1-1/20230618_100636_standard_comp_to_omission_D2_subj_1-4_and_1-1.1.fixed.2_subj.round_1.id_corrected.h5</t>
+  </si>
+  <si>
+    <t>/scratch/back_up/reward_competition_extention/final_proc/id_corrected/20230618_100636_standard_comp_to_omission_D2_subj_1-4_and_1-1/20230618_100636_standard_comp_to_omission_D2_subj_1-4_and_1-1.2.fixed.1_subj.round_1.id_corrected.h5</t>
+  </si>
+  <si>
+    <t>/scratch/back_up/reward_competition_extention/final_proc/id_corrected/20230619_115321_standard_comp_to_omission_D3_subj_1-2_and_1-4/20230619_115321_standard_comp_to_omission_D3_subj_1-2_and_1-4.3.fixed.1_subj.round_1.id_corrected.h5</t>
   </si>
   <si>
     <t>1.2_1.4</t>
   </si>
   <si>
-    <t>/scratch/back_up/reward_competition_extention/proc/id_corrected/20230619_115321_standard_comp_to_omission_D3_subj_1-2_and_1-4/20230619_115321_standard_comp_to_omission_D3_subj_1-2_and_1-4.3.fixed.2_subj.round_1.id_corrected.h5</t>
-  </si>
-  <si>
-    <t>/scratch/back_up/reward_competition_extention/proc/id_corrected/20230619_115321_standard_comp_to_omission_D3_subj_1-2_and_1-4/20230619_115321_standard_comp_to_omission_D3_subj_1-2_and_1-4.4.fixed.1_subj.round_1.id_corrected.h5</t>
-  </si>
-  <si>
-    <t>/scratch/back_up/reward_competition_extention/proc/id_corrected/20230620_114347_standard_comp_to_omission_D4_subj_1-2_and_1-1/20230620_114347_standard_comp_to_omission_D4_subj_1-2_and_1-1.1.fixed.1_subj.round_1.id_corrected.h5</t>
-  </si>
-  <si>
-    <t>/scratch/back_up/reward_competition_extention/proc/id_corrected/20230620_114347_standard_comp_to_omission_D4_subj_1-2_and_1-1/20230620_114347_standard_comp_to_omission_D4_subj_1-2_and_1-1.1.fixed.2_subj.round_1.id_corrected.h5</t>
-  </si>
-  <si>
-    <t>/scratch/back_up/reward_competition_extention/proc/id_corrected/20230620_114347_standard_comp_to_omission_D4_subj_1-2_and_1-1/20230620_114347_standard_comp_to_omission_D4_subj_1-2_and_1-1.2.fixed.1_subj.round_1.id_corrected.h5</t>
-  </si>
-  <si>
-    <t>/scratch/back_up/reward_competition_extention/proc/id_corrected/20230621_111240_standard_comp_to_omission_D5_subj_1-4_and_1-2/20230621_111240_standard_comp_to_omission_D5_subj_1-4_and_1-2.1.fixed.1_subj.round_1.id_corrected.h5</t>
-  </si>
-  <si>
-    <t>/scratch/back_up/reward_competition_extention/proc/id_corrected/20230621_111240_standard_comp_to_omission_D5_subj_1-4_and_1-2/20230621_111240_standard_comp_to_omission_D5_subj_1-4_and_1-2.1.fixed.2_subj.round_1.id_corrected.h5</t>
-  </si>
-  <si>
-    <t>/scratch/back_up/reward_competition_extention/proc/id_corrected/20230621_111240_standard_comp_to_omission_D5_subj_1-4_and_1-2/20230621_111240_standard_comp_to_omission_D5_subj_1-4_and_1-2.2.fixed.1_subj.round_1.id_corrected.h5</t>
+    <t>/scratch/back_up/reward_competition_extention/final_proc/id_corrected/20230619_115321_standard_comp_to_omission_D3_subj_1-2_and_1-4/20230619_115321_standard_comp_to_omission_D3_subj_1-2_and_1-4.3.fixed.2_subj.round_1.id_corrected.h5</t>
+  </si>
+  <si>
+    <t>/scratch/back_up/reward_competition_extention/final_proc/id_corrected/20230619_115321_standard_comp_to_omission_D3_subj_1-2_and_1-4/20230619_115321_standard_comp_to_omission_D3_subj_1-2_and_1-4.4.fixed.1_subj.round_1.id_corrected.h5</t>
+  </si>
+  <si>
+    <t>/scratch/back_up/reward_competition_extention/final_proc/id_corrected/20230620_114347_standard_comp_to_omission_D4_subj_1-2_and_1-1/20230620_114347_standard_comp_to_omission_D4_subj_1-2_and_1-1.1.fixed.1_subj.round_1.id_corrected.h5</t>
+  </si>
+  <si>
+    <t>/scratch/back_up/reward_competition_extention/final_proc/id_corrected/20230620_114347_standard_comp_to_omission_D4_subj_1-2_and_1-1/20230620_114347_standard_comp_to_omission_D4_subj_1-2_and_1-1.1.fixed.2_subj.round_1.id_corrected.h5</t>
+  </si>
+  <si>
+    <t>/scratch/back_up/reward_competition_extention/final_proc/id_corrected/20230620_114347_standard_comp_to_omission_D4_subj_1-2_and_1-1/20230620_114347_standard_comp_to_omission_D4_subj_1-2_and_1-1.2.fixed.1_subj.round_1.id_corrected.h5</t>
+  </si>
+  <si>
+    <t>/scratch/back_up/reward_competition_extention/final_proc/id_corrected/20230621_111240_standard_comp_to_omission_D5_subj_1-4_and_1-2/20230621_111240_standard_comp_to_omission_D5_subj_1-4_and_1-2.1.fixed.1_subj.round_1.id_corrected.h5</t>
+  </si>
+  <si>
+    <t>/scratch/back_up/reward_competition_extention/final_proc/id_corrected/20230621_111240_standard_comp_to_omission_D5_subj_1-4_and_1-2/20230621_111240_standard_comp_to_omission_D5_subj_1-4_and_1-2.1.fixed.2_subj.round_1.id_corrected.h5</t>
+  </si>
+  <si>
+    <t>/scratch/back_up/reward_competition_extention/final_proc/id_corrected/20230621_111240_standard_comp_to_omission_D5_subj_1-4_and_1-2/20230621_111240_standard_comp_to_omission_D5_subj_1-4_and_1-2.2.fixed.1_subj.round_1.id_corrected.h5</t>
   </si>
   <si>
     <t>/scratch/back_up/reward_competition_extention/final_proc/id_corrected/20230612_112630_standard_comp_to_training_D1_subj_1-2_and_1-1/20230612_112630_standard_comp_to_training_D1_subj_1-2_and_1-1.1.1_subj.id_corrected.h5</t>
@@ -166,7 +166,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -181,6 +181,11 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
     </font>
   </fonts>
   <fills count="3">
@@ -209,16 +214,21 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -536,8 +546,8 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A24" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E2" sqref="E2"/>
+      <pane ySplit="1" topLeftCell="A30" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C24" sqref="C24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -598,7 +608,7 @@
         <v>27500</v>
       </c>
       <c r="C4" s="1">
-        <v>73601</v>
+        <v>73600</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>7</v>
@@ -615,7 +625,7 @@
         <v>51500</v>
       </c>
       <c r="C5" s="1">
-        <v>76455</v>
+        <v>76454</v>
       </c>
       <c r="D5" s="1">
         <v>6.3</v>
@@ -649,7 +659,7 @@
         <v>41000</v>
       </c>
       <c r="C7" s="1">
-        <v>79051</v>
+        <v>79050</v>
       </c>
       <c r="D7" s="1">
         <v>1.1000000000000001</v>
@@ -663,7 +673,7 @@
         <v>13</v>
       </c>
       <c r="B8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C8" s="1">
         <v>39500</v>
@@ -680,7 +690,7 @@
         <v>14</v>
       </c>
       <c r="B9" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C9" s="1">
         <v>38957</v>
@@ -700,7 +710,7 @@
         <v>32792</v>
       </c>
       <c r="C10" s="1">
-        <v>68495</v>
+        <v>68494</v>
       </c>
       <c r="D10" s="1">
         <v>1.4</v>
@@ -714,7 +724,7 @@
         <v>17</v>
       </c>
       <c r="B11" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C11" s="1">
         <v>32316</v>
@@ -734,7 +744,7 @@
         <v>32792</v>
       </c>
       <c r="C12" s="1">
-        <v>68495</v>
+        <v>68494</v>
       </c>
       <c r="D12" s="1">
         <v>1.1000000000000001</v>
@@ -758,7 +768,7 @@
         <v>32500</v>
       </c>
       <c r="C14" s="1">
-        <v>66320</v>
+        <v>66319</v>
       </c>
       <c r="D14" s="1">
         <v>1.2</v>
@@ -772,7 +782,7 @@
         <v>21</v>
       </c>
       <c r="B15" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C15" s="1">
         <v>30000</v>
@@ -792,7 +802,7 @@
         <v>32500</v>
       </c>
       <c r="C16" s="1">
-        <v>66006</v>
+        <v>66005</v>
       </c>
       <c r="D16" s="1">
         <v>1.4</v>
@@ -801,14 +811,14 @@
         <v>20</v>
       </c>
     </row>
-    <row r="17" spans="1:5" s="2" customFormat="1">
+    <row r="17" spans="1:6" s="2" customFormat="1">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
     </row>
-    <row r="18" spans="1:5" s="2" customFormat="1" ht="76.5">
+    <row r="18" spans="1:6" s="2" customFormat="1" ht="76.5">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
@@ -816,7 +826,7 @@
         <v>32860</v>
       </c>
       <c r="C18" s="1">
-        <v>68288</v>
+        <v>68287</v>
       </c>
       <c r="D18" s="1">
         <v>1.2</v>
@@ -825,7 +835,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="19" spans="1:5" s="2" customFormat="1" ht="76.5">
+    <row r="19" spans="1:6" s="2" customFormat="1" ht="76.5">
       <c r="A19" s="1" t="s">
         <v>24</v>
       </c>
@@ -833,7 +843,7 @@
         <v>2027</v>
       </c>
       <c r="C19" s="1">
-        <v>32240</v>
+        <v>32239</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>12</v>
@@ -842,7 +852,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:5" s="2" customFormat="1" ht="76.5">
+    <row r="20" spans="1:6" s="2" customFormat="1" ht="76.5">
       <c r="A20" s="1" t="s">
         <v>25</v>
       </c>
@@ -850,7 +860,7 @@
         <v>32860</v>
       </c>
       <c r="C20" s="1">
-        <v>68288</v>
+        <v>68287</v>
       </c>
       <c r="D20" s="1">
         <v>1.1000000000000001</v>
@@ -859,288 +869,302 @@
         <v>12</v>
       </c>
     </row>
-    <row r="21" spans="1:5" s="2" customFormat="1">
+    <row r="21" spans="1:6" s="2" customFormat="1">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
     </row>
-    <row r="22" spans="1:5" ht="76.5">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:6" ht="76.5">
+      <c r="A22" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B22">
+      <c r="B22" s="5">
         <v>35000</v>
       </c>
-      <c r="C22">
-        <v>69768</v>
-      </c>
-      <c r="D22">
+      <c r="C22" s="5">
+        <v>69766</v>
+      </c>
+      <c r="D22" s="5">
         <v>1.4</v>
       </c>
-      <c r="E22" t="s">
+      <c r="E22" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:5" ht="76.5">
-      <c r="A23" s="1" t="s">
+      <c r="F22" s="5"/>
+    </row>
+    <row r="23" spans="1:6" ht="76.5">
+      <c r="A23" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="B23">
+      <c r="B23" s="5">
         <v>1</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="5">
         <v>33500</v>
       </c>
-      <c r="D23" t="s">
+      <c r="D23" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="E23" t="s">
+      <c r="E23" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="24" spans="1:5" ht="76.5">
-      <c r="A24" s="1" t="s">
+      <c r="F23" s="5"/>
+    </row>
+    <row r="24" spans="1:6" ht="76.5">
+      <c r="A24" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="B24">
+      <c r="B24" s="5">
         <v>34500</v>
       </c>
-      <c r="C24">
-        <v>69684</v>
-      </c>
-      <c r="D24">
+      <c r="C24" s="5">
+        <v>69683</v>
+      </c>
+      <c r="D24" s="5">
         <v>1.2</v>
       </c>
-      <c r="E24" t="s">
+      <c r="E24" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="25" spans="1:5" s="4" customFormat="1" ht="60.75">
-      <c r="A25" s="3" t="s">
+      <c r="F24" s="5"/>
+    </row>
+    <row r="25" spans="1:6" s="3" customFormat="1" ht="60.75">
+      <c r="A25" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="B25" s="4">
+      <c r="B25" s="7">
         <v>32700</v>
       </c>
-      <c r="C25" s="4">
+      <c r="C25" s="7">
         <v>68257</v>
       </c>
-      <c r="D25" s="4">
+      <c r="D25" s="7">
         <v>1.2</v>
       </c>
-      <c r="E25" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="26" spans="1:5" s="4" customFormat="1" ht="60.75">
-      <c r="A26" s="3" t="s">
+      <c r="E25" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F25" s="7"/>
+    </row>
+    <row r="26" spans="1:6" s="3" customFormat="1" ht="60.75">
+      <c r="A26" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="B26" s="4">
+      <c r="B26" s="7">
         <v>1</v>
       </c>
-      <c r="C26" s="4">
+      <c r="C26" s="7">
         <v>32300</v>
       </c>
-      <c r="D26" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="27" spans="1:5" s="4" customFormat="1" ht="60.75">
-      <c r="A27" s="3" t="s">
+      <c r="D26" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F26" s="7"/>
+    </row>
+    <row r="27" spans="1:6" s="3" customFormat="1" ht="60.75">
+      <c r="A27" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B27" s="4">
+      <c r="B27" s="7">
         <v>33000</v>
       </c>
-      <c r="C27" s="4">
+      <c r="C27" s="7">
         <v>68212</v>
       </c>
-      <c r="D27" s="4">
+      <c r="D27" s="7">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E27" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="28" spans="1:5" s="4" customFormat="1" ht="60.75">
-      <c r="A28" s="3" t="s">
+      <c r="E27" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F27" s="7"/>
+    </row>
+    <row r="28" spans="1:6" s="3" customFormat="1" ht="60.75">
+      <c r="A28" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="B28" s="4">
+      <c r="B28" s="7">
         <v>33400</v>
       </c>
-      <c r="C28" s="4">
+      <c r="C28" s="7">
         <v>68332</v>
       </c>
-      <c r="D28" s="4">
+      <c r="D28" s="7">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E28" s="4" t="s">
+      <c r="E28" s="7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="29" spans="1:5" s="4" customFormat="1" ht="60.75">
-      <c r="A29" s="3" t="s">
+      <c r="F28" s="7"/>
+    </row>
+    <row r="29" spans="1:6" s="3" customFormat="1" ht="60.75">
+      <c r="A29" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="B29" s="4">
+      <c r="B29" s="7">
         <v>1</v>
       </c>
-      <c r="C29" s="4">
+      <c r="C29" s="7">
         <v>33000</v>
       </c>
-      <c r="D29" s="4" t="s">
+      <c r="D29" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="E29" s="4" t="s">
+      <c r="E29" s="7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="30" spans="1:5" s="4" customFormat="1" ht="60.75">
-      <c r="A30" s="3" t="s">
+      <c r="F29" s="7"/>
+    </row>
+    <row r="30" spans="1:6" s="3" customFormat="1" ht="60.75">
+      <c r="A30" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="B30" s="4">
+      <c r="B30" s="7">
         <v>33700</v>
       </c>
-      <c r="C30" s="4">
+      <c r="C30" s="7">
         <v>68292</v>
       </c>
-      <c r="D30" s="4">
+      <c r="D30" s="7">
         <v>1.4</v>
       </c>
-      <c r="E30" s="4" t="s">
+      <c r="E30" s="7" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="31" spans="1:5" s="4" customFormat="1" ht="60.75">
-      <c r="A31" s="3" t="s">
+      <c r="F30" s="7"/>
+    </row>
+    <row r="31" spans="1:6" s="3" customFormat="1" ht="60.75">
+      <c r="A31" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="B31" s="4">
+      <c r="B31" s="7">
         <v>32800</v>
       </c>
-      <c r="C31" s="4">
+      <c r="C31" s="7">
         <v>44205</v>
       </c>
-      <c r="D31" s="4">
+      <c r="D31" s="7">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E31" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="32" spans="1:5" s="4" customFormat="1" ht="60.75">
-      <c r="A32" s="3" t="s">
+      <c r="E31" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F31" s="7"/>
+    </row>
+    <row r="32" spans="1:6" s="3" customFormat="1" ht="60.75">
+      <c r="A32" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B32" s="4">
+      <c r="B32" s="7">
         <v>1</v>
       </c>
-      <c r="C32" s="4">
+      <c r="C32" s="7">
         <v>32200</v>
       </c>
-      <c r="D32" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" s="4" customFormat="1" ht="60.75">
-      <c r="A33" s="3" t="s">
+      <c r="D32" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="E32" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F32" s="7"/>
+    </row>
+    <row r="33" spans="1:6" s="3" customFormat="1" ht="60.75">
+      <c r="A33" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="B33" s="4">
+      <c r="B33" s="7">
         <v>41600</v>
       </c>
-      <c r="C33" s="4">
+      <c r="C33" s="7">
         <v>75829</v>
       </c>
-      <c r="D33" s="4">
+      <c r="D33" s="7">
         <v>1.2</v>
       </c>
-      <c r="E33" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="F33" s="4" t="s">
+      <c r="E33" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F33" s="7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="34" spans="1:6" s="4" customFormat="1" ht="60.75">
-      <c r="A34" s="3" t="s">
+    <row r="34" spans="1:6" s="3" customFormat="1" ht="60.75">
+      <c r="A34" s="6" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="4">
+      <c r="B34" s="7">
         <v>1</v>
       </c>
-      <c r="C34" s="4">
+      <c r="C34" s="7">
         <v>23574</v>
       </c>
-      <c r="D34" s="4">
+      <c r="D34" s="7">
         <v>1.1000000000000001</v>
       </c>
-      <c r="E34" s="4" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" s="4" customFormat="1" ht="60.75">
-      <c r="A35" s="3" t="s">
+      <c r="E34" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="F34" s="7"/>
+    </row>
+    <row r="35" spans="1:6" s="3" customFormat="1" ht="60.75">
+      <c r="A35" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="4">
+      <c r="B35" s="7">
         <v>32100</v>
       </c>
-      <c r="C35" s="4">
+      <c r="C35" s="7">
         <v>67369</v>
       </c>
-      <c r="D35" s="4">
+      <c r="D35" s="7">
         <v>1.4</v>
       </c>
-      <c r="E35" s="4" t="s">
+      <c r="E35" s="7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="36" spans="1:6" s="4" customFormat="1" ht="60.75">
-      <c r="A36" s="3" t="s">
+      <c r="F35" s="7"/>
+    </row>
+    <row r="36" spans="1:6" s="3" customFormat="1" ht="60.75">
+      <c r="A36" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="4">
+      <c r="B36" s="7">
         <v>1</v>
       </c>
-      <c r="C36" s="4">
+      <c r="C36" s="7">
         <v>31100</v>
       </c>
-      <c r="D36" s="4" t="s">
+      <c r="D36" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E36" s="4" t="s">
+      <c r="E36" s="7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="37" spans="1:6" s="4" customFormat="1" ht="60.75">
-      <c r="A37" s="3" t="s">
+      <c r="F36" s="7"/>
+    </row>
+    <row r="37" spans="1:6" s="3" customFormat="1" ht="60.75">
+      <c r="A37" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="B37" s="4">
+      <c r="B37" s="7">
         <v>36100</v>
       </c>
-      <c r="C37" s="4">
+      <c r="C37" s="7">
         <v>71644</v>
       </c>
-      <c r="D37" s="4">
+      <c r="D37" s="7">
         <v>1.2</v>
       </c>
-      <c r="E37" s="4" t="s">
+      <c r="E37" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="F37" s="4" t="s">
+      <c r="F37" s="7" t="s">
         <v>38</v>
       </c>
     </row>
@@ -1405,6 +1429,15 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <TaxCatchAll xmlns="66c7fa70-bb82-47de-8c9f-8b3ecea6303f" xsi:nil="true"/>
@@ -1415,23 +1448,14 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{6A2E4F11-7516-4015-A04F-C6297B95747E}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AE888698-F550-4D99-B643-806A083D1CEB}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D770834-2B26-4F25-8CBB-FA13B41D6738}"/>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{2D770834-2B26-4F25-8CBB-FA13B41D6738}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AE888698-F550-4D99-B643-806A083D1CEB}"/>
 </file>
</xml_diff>